<commit_message>
Add Low Rule Interpolation
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NewVEDA\Veda_models\Demo_models\DemoS_009\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JULIAN\Desktop\DEMO_009\Demo_009_TIMES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B35FF3-FB9E-4A9B-9317-4FC00CFF392D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF29E09-3EC2-4BB5-878D-0011DC4D64A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="853" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="853" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Region-Time Slices" sheetId="16" r:id="rId1"/>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="123">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -495,6 +495,9 @@
   </si>
   <si>
     <t>Twh</t>
+  </si>
+  <si>
+    <t>UP,LO</t>
   </si>
 </sst>
 </file>
@@ -856,7 +859,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1019,6 +1022,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3568,16 +3572,16 @@
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.140625" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="7" max="7" width="3.42578125" customWidth="1"/>
-    <col min="8" max="8" width="29.42578125" customWidth="1"/>
+    <col min="1" max="1" width="2.109375" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="7" max="7" width="3.44140625" customWidth="1"/>
+    <col min="8" max="8" width="29.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -3588,7 +3592,7 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="2" t="s">
         <v>15</v>
@@ -3606,7 +3610,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="17" t="s">
         <v>50</v>
@@ -3622,7 +3626,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="17" t="s">
         <v>79</v>
@@ -3638,126 +3642,126 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
     </row>
   </sheetData>
@@ -3778,42 +3782,42 @@
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>2005</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="15" t="s">
         <v>36</v>
       </c>
@@ -3824,7 +3828,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="16">
         <v>1</v>
       </c>
@@ -3835,7 +3839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="16">
         <v>2</v>
       </c>
@@ -3846,7 +3850,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="16"/>
       <c r="C15" s="16">
         <v>5</v>
@@ -3855,7 +3859,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="16"/>
       <c r="C16" s="16">
         <v>5</v>
@@ -3864,7 +3868,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="16"/>
       <c r="C17" s="16">
         <v>5</v>
@@ -3873,42 +3877,42 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
       <c r="D19" s="16">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
       <c r="D20" s="16">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
       <c r="D23" s="16">
@@ -3932,18 +3936,18 @@
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.42578125" customWidth="1"/>
-    <col min="2" max="2" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.44140625" customWidth="1"/>
+    <col min="2" max="2" width="52.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
         <v>28</v>
       </c>
@@ -3951,7 +3955,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="2:3" s="74" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:3" s="74" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="76" t="s">
         <v>30</v>
       </c>
@@ -3959,7 +3963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="77" t="s">
         <v>31</v>
       </c>
@@ -3967,7 +3971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
         <v>32</v>
       </c>
@@ -3975,7 +3979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
         <v>33</v>
       </c>
@@ -3983,7 +3987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="16" t="s">
         <v>81</v>
       </c>
@@ -4004,27 +4008,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B3:F37"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34:E37"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.7109375" customWidth="1"/>
-    <col min="13" max="13" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" width="2.88671875" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.6640625" customWidth="1"/>
+    <col min="13" max="13" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
@@ -4034,16 +4038,16 @@
       <c r="D4" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="82" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>82</v>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="20" t="s">
+        <v>122</v>
       </c>
       <c r="C5" t="s">
         <v>83</v>
@@ -4055,7 +4059,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>82</v>
       </c>
@@ -4069,7 +4073,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>82</v>
       </c>
@@ -4083,26 +4087,26 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B30" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="2:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B32" s="9" t="s">
         <v>40</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="5" t="s">
         <v>21</v>
       </c>
@@ -4116,7 +4120,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>3</v>
       </c>
@@ -4130,7 +4134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>3</v>
       </c>
@@ -4161,28 +4165,28 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="12"/>
-    <col min="2" max="2" width="12.140625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="12" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="12"/>
+    <col min="2" max="2" width="12.109375" style="12" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" style="12" customWidth="1"/>
     <col min="4" max="4" width="14" style="12" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="12" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="12"/>
+    <col min="5" max="5" width="10.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" style="12" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="12"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>19</v>
       </c>
@@ -4205,7 +4209,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D7" s="12" t="s">
         <v>52</v>
       </c>
@@ -4215,7 +4219,7 @@
       <c r="F7" s="18"/>
       <c r="G7" s="18"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D8" s="12" t="s">
         <v>42</v>
       </c>
@@ -4225,7 +4229,7 @@
       <c r="F8" s="18"/>
       <c r="G8" s="18"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="72" t="s">
         <v>59</v>
       </c>
@@ -4238,7 +4242,7 @@
         <v>0.24971461187214614</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="72" t="s">
         <v>60</v>
       </c>
@@ -4251,7 +4255,7 @@
         <v>0.22973744292237441</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="72" t="s">
         <v>61</v>
       </c>
@@ -4264,7 +4268,7 @@
         <v>0.24942922374429224</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="72" t="s">
         <v>62</v>
       </c>
@@ -4277,7 +4281,7 @@
         <v>0.27111872146118721</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13"/>
       <c r="C13"/>
       <c r="D13" s="18" t="s">
@@ -4294,7 +4298,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14"/>
       <c r="C14"/>
       <c r="D14" s="18"/>
@@ -4302,7 +4306,7 @@
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15"/>
       <c r="C15"/>
       <c r="D15" s="18"/>
@@ -4310,7 +4314,7 @@
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
@@ -4318,7 +4322,7 @@
       <c r="F16" s="18"/>
       <c r="G16" s="18"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17"/>
       <c r="C17"/>
       <c r="D17"/>
@@ -4326,7 +4330,7 @@
       <c r="F17" s="18"/>
       <c r="G17" s="18"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18"/>
       <c r="C18"/>
       <c r="D18"/>
@@ -4334,7 +4338,7 @@
       <c r="F18" s="18"/>
       <c r="G18" s="18"/>
     </row>
-    <row r="19" spans="2:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B19" s="23" t="s">
         <v>58</v>
       </c>
@@ -4344,14 +4348,14 @@
       <c r="F19" s="25"/>
       <c r="G19" s="25"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="26"/>
       <c r="C20" s="27"/>
       <c r="D20" s="27"/>
       <c r="E20" s="28"/>
       <c r="F20" s="28"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="29" t="s">
         <v>21</v>
       </c>
@@ -4368,7 +4372,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="24" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:7" ht="24" x14ac:dyDescent="0.25">
       <c r="B22" s="33"/>
       <c r="C22" s="34" t="s">
         <v>63</v>
@@ -4383,7 +4387,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="29" t="s">
         <v>51</v>
       </c>
@@ -4408,14 +4412,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="41"/>
       <c r="C24" s="41"/>
       <c r="D24" s="41"/>
       <c r="E24" s="42"/>
       <c r="F24" s="42"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="42"/>
       <c r="C25" s="43"/>
       <c r="D25" s="43"/>
@@ -4423,7 +4427,7 @@
       <c r="F25" s="41"/>
       <c r="G25" s="44"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="44"/>
       <c r="C26" s="45" t="s">
         <v>67</v>
@@ -4437,7 +4441,7 @@
       <c r="F26" s="48"/>
       <c r="G26" s="44"/>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="49" t="s">
         <v>70</v>
       </c>
@@ -4454,7 +4458,7 @@
       <c r="F27" s="53"/>
       <c r="G27" s="44"/>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="54" t="s">
         <v>72</v>
       </c>
@@ -4472,7 +4476,7 @@
       <c r="F28" s="53"/>
       <c r="G28" s="44"/>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="42"/>
       <c r="C29" s="44"/>
       <c r="D29" s="58">
@@ -4486,7 +4490,7 @@
       <c r="F29" s="60"/>
       <c r="G29" s="44"/>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="42"/>
       <c r="C30" s="44"/>
       <c r="D30" s="61"/>
@@ -4494,7 +4498,7 @@
       <c r="F30" s="44"/>
       <c r="G30" s="44"/>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="62"/>
       <c r="C31" s="63" t="s">
         <v>74</v>
@@ -4506,7 +4510,7 @@
       <c r="F31" s="44"/>
       <c r="G31" s="44"/>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="65" t="s">
         <v>71</v>
       </c>
@@ -4523,7 +4527,7 @@
       </c>
       <c r="G32" s="44"/>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="69" t="s">
         <v>76</v>
       </c>
@@ -4553,21 +4557,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B2:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>44</v>
       </c>
@@ -4575,7 +4579,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="13" t="s">
         <v>45</v>
       </c>
@@ -4598,7 +4602,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
         <v>93</v>
       </c>
@@ -4621,7 +4625,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="6"/>
       <c r="D5" t="s">
         <v>48</v>
@@ -4642,7 +4646,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
       <c r="D6" t="s">
         <v>49</v>
@@ -4663,15 +4667,15 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>97</v>
       </c>
@@ -4682,7 +4686,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>100</v>
       </c>
@@ -4693,7 +4697,7 @@
         <v>1055.55</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>101</v>
       </c>
@@ -4704,7 +4708,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>102</v>
       </c>
@@ -4715,7 +4719,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>104</v>
       </c>
@@ -4726,7 +4730,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>106</v>
       </c>
@@ -4737,7 +4741,7 @@
         <v>1.05555</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>107</v>
       </c>
@@ -4748,7 +4752,7 @@
         <v>4.1868000000000002E-2</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>108</v>
       </c>
@@ -4759,7 +4763,7 @@
         <v>41.868000000000002</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>109</v>
       </c>
@@ -4770,7 +4774,7 @@
         <v>3.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>110</v>
       </c>
@@ -4781,7 +4785,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>111</v>
       </c>
@@ -4792,7 +4796,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>113</v>
       </c>
@@ -4803,7 +4807,7 @@
         <v>0.15384600000000001</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>115</v>
       </c>
@@ -4814,7 +4818,7 @@
         <v>-1E-3</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>117</v>
       </c>
@@ -4825,7 +4829,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>118</v>
       </c>
@@ -4836,7 +4840,7 @@
         <v>37.681199999999997</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>119</v>
       </c>
@@ -4847,7 +4851,7 @@
         <v>2299</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>120</v>
       </c>
@@ -4858,7 +4862,7 @@
         <v>2.7777769999999999</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>121</v>
       </c>
@@ -4869,7 +4873,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>53</v>
       </c>
@@ -4895,18 +4899,18 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.28515625" customWidth="1"/>
-    <col min="9" max="11" width="11.85546875" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.33203125" customWidth="1"/>
+    <col min="9" max="11" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -4915,7 +4919,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="2:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
         <v>37</v>
       </c>
@@ -4926,7 +4930,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="4" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
@@ -4935,12 +4939,12 @@
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
     </row>
-    <row r="5" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
@@ -4966,7 +4970,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="10" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
Subida archivos de TIMESOG
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -1,28 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JULIAN\Desktop\DEMO_009\Demo_009_TIMES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JULIAN\Pictures\TIMES-O-G-B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF897C5-9A58-447C-BE28-1FBAE8E68CAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C61749-86E6-4D7A-90DE-CC8705FCF610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="853" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="853" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Region-Time Slices" sheetId="16" r:id="rId1"/>
     <sheet name="TimePeriods" sheetId="18" r:id="rId2"/>
-    <sheet name="Import Settings" sheetId="17" r:id="rId3"/>
-    <sheet name="Interpol_Extrapol_Defaults" sheetId="14" r:id="rId4"/>
-    <sheet name="Constants" sheetId="20" r:id="rId5"/>
-    <sheet name="Defaults" sheetId="21" r:id="rId6"/>
-    <sheet name="Commodity Group" sheetId="15" r:id="rId7"/>
+    <sheet name="Interpol_Extrapol_Defaults" sheetId="14" r:id="rId3"/>
+    <sheet name="Constants" sheetId="20" r:id="rId4"/>
+    <sheet name="Defaults" sheetId="21" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId8"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
     <definedName name="FID_1">[1]AGR_Fuels!$A$2</definedName>
@@ -65,71 +63,8 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Maurizio Gargiulo</author>
-  </authors>
-  <commentList>
-    <comment ref="G6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Possible definitions
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Y </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">or a </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>positive number</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (mean apply this User CG in that region)
-Empty mean this User CG is not applied in that region</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="116">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -146,18 +81,6 @@
     <t>IMPDEMZ</t>
   </si>
   <si>
-    <t>User-Defined CG</t>
-  </si>
-  <si>
-    <t>~TFM_COMGRP</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>~BookRegions_Map</t>
   </si>
   <si>
@@ -203,36 +126,12 @@
     <t>Pset_PN</t>
   </si>
   <si>
-    <t>Cset_Set</t>
-  </si>
-  <si>
     <t>Cset_CN</t>
   </si>
   <si>
-    <t>Cset_CD</t>
-  </si>
-  <si>
-    <t>~ImpSettings</t>
-  </si>
-  <si>
     <t>Option</t>
   </si>
   <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Check #DIV/0 and #REF errors in Templates</t>
-  </si>
-  <si>
-    <t>Create Dummy Imports for Energy and Material Commodities</t>
-  </si>
-  <si>
-    <t>Create Dummy Imports for Demands</t>
-  </si>
-  <si>
-    <t>Generate Vintage Bounds</t>
-  </si>
-  <si>
     <t>~StartYear</t>
   </si>
   <si>
@@ -242,15 +141,6 @@
     <t>Pdef-1</t>
   </si>
   <si>
-    <t>* Define the explicit commodity groups needed</t>
-  </si>
-  <si>
-    <t>\I:Commodity Group Name</t>
-  </si>
-  <si>
-    <t>Commodity Group Description</t>
-  </si>
-  <si>
     <t>Dummy Imp Prices</t>
   </si>
   <si>
@@ -299,12 +189,6 @@
     <t>Pja</t>
   </si>
   <si>
-    <t>COM_IE</t>
-  </si>
-  <si>
-    <t>ELC</t>
-  </si>
-  <si>
     <t>Time slices</t>
   </si>
   <si>
@@ -362,142 +246,172 @@
     <t>W</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>REG2</t>
   </si>
   <si>
     <t>Pdef-5</t>
   </si>
   <si>
-    <t>DumVarforUC</t>
-  </si>
-  <si>
-    <t>UP</t>
-  </si>
-  <si>
     <t>ACT_BND</t>
   </si>
   <si>
+    <t>~TFM_MIG</t>
+  </si>
+  <si>
+    <t>Year2</t>
+  </si>
+  <si>
+    <t>~UnitConversion</t>
+  </si>
+  <si>
+    <t>from_unit</t>
+  </si>
+  <si>
+    <t>to_unit</t>
+  </si>
+  <si>
+    <t>multiplier</t>
+  </si>
+  <si>
+    <t>QBtu</t>
+  </si>
+  <si>
+    <t>Billion Kwh</t>
+  </si>
+  <si>
+    <t>Mt</t>
+  </si>
+  <si>
+    <t>Kt</t>
+  </si>
+  <si>
+    <t>B Euro</t>
+  </si>
+  <si>
+    <t>M Euro</t>
+  </si>
+  <si>
+    <t>TBtu</t>
+  </si>
+  <si>
+    <t>ktoe</t>
+  </si>
+  <si>
+    <t>mtoe</t>
+  </si>
+  <si>
+    <t>Gwh</t>
+  </si>
+  <si>
+    <t>Gt</t>
+  </si>
+  <si>
+    <t>bEur</t>
+  </si>
+  <si>
+    <t>mEur</t>
+  </si>
+  <si>
+    <t>Eur per bbl</t>
+  </si>
+  <si>
+    <t>Eur per GJ</t>
+  </si>
+  <si>
+    <t>Eur per ton</t>
+  </si>
+  <si>
+    <t>mEur per kt</t>
+  </si>
+  <si>
+    <t>EJ</t>
+  </si>
+  <si>
+    <t>bcm</t>
+  </si>
+  <si>
+    <t>mbpd</t>
+  </si>
+  <si>
+    <t>Cents per Kwh</t>
+  </si>
+  <si>
+    <t>Twh</t>
+  </si>
+  <si>
     <t>Share-O</t>
   </si>
   <si>
     <t>Share-I</t>
   </si>
   <si>
+    <t>Pdef-6</t>
+  </si>
+  <si>
     <t>Pdef-11</t>
   </si>
   <si>
-    <t>GW</t>
-  </si>
-  <si>
-    <t>IND</t>
-  </si>
-  <si>
-    <t>RCA</t>
-  </si>
-  <si>
-    <t>TRA</t>
-  </si>
-  <si>
-    <t>kPk</t>
-  </si>
-  <si>
-    <t>000_Units</t>
-  </si>
-  <si>
-    <t>MEuro05</t>
-  </si>
-  <si>
-    <t>~TFM_MIG</t>
-  </si>
-  <si>
-    <t>Year2</t>
-  </si>
-  <si>
-    <t>~UnitConversion</t>
-  </si>
-  <si>
-    <t>from_unit</t>
-  </si>
-  <si>
-    <t>to_unit</t>
-  </si>
-  <si>
-    <t>multiplier</t>
-  </si>
-  <si>
-    <t>QBtu</t>
-  </si>
-  <si>
-    <t>Billion Kwh</t>
-  </si>
-  <si>
-    <t>Mt</t>
-  </si>
-  <si>
-    <t>Kt</t>
-  </si>
-  <si>
-    <t>B Euro</t>
-  </si>
-  <si>
-    <t>M Euro</t>
-  </si>
-  <si>
-    <t>TBtu</t>
-  </si>
-  <si>
-    <t>ktoe</t>
-  </si>
-  <si>
-    <t>mtoe</t>
-  </si>
-  <si>
-    <t>Gwh</t>
-  </si>
-  <si>
-    <t>Gt</t>
-  </si>
-  <si>
-    <t>bEur</t>
-  </si>
-  <si>
-    <t>mEur</t>
-  </si>
-  <si>
-    <t>Eur per bbl</t>
-  </si>
-  <si>
-    <t>Eur per GJ</t>
-  </si>
-  <si>
-    <t>Eur per ton</t>
-  </si>
-  <si>
-    <t>mEur per kt</t>
-  </si>
-  <si>
-    <t>EJ</t>
-  </si>
-  <si>
-    <t>bcm</t>
-  </si>
-  <si>
-    <t>mbpd</t>
-  </si>
-  <si>
-    <t>Cents per Kwh</t>
-  </si>
-  <si>
-    <t>Twh</t>
-  </si>
-  <si>
-    <t>UP,LO</t>
+    <t>Pdef-24</t>
+  </si>
+  <si>
+    <t>pdef-100</t>
+  </si>
+  <si>
+    <t>pdef-200</t>
+  </si>
+  <si>
+    <t>Pdef-100</t>
+  </si>
+  <si>
+    <t>~Milestoneyears</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>endyear</t>
+  </si>
+  <si>
+    <t>milestoneyear</t>
+  </si>
+  <si>
+    <t>msy3_2025</t>
+  </si>
+  <si>
+    <t>prueba_2025</t>
+  </si>
+  <si>
+    <t>UP, FX</t>
+  </si>
+  <si>
+    <t>prueba_2040</t>
+  </si>
+  <si>
+    <t>EFF</t>
+  </si>
+  <si>
+    <t>TOTAL_2040</t>
+  </si>
+  <si>
+    <t>UP, FX, LO</t>
+  </si>
+  <si>
+    <t>prueba_2050</t>
+  </si>
+  <si>
+    <t>total_2050</t>
+  </si>
+  <si>
+    <t>ANNUAL</t>
+  </si>
+  <si>
+    <t>MUSD19</t>
+  </si>
+  <si>
+    <t>STOCK</t>
+  </si>
+  <si>
+    <t>fivestep</t>
   </si>
 </sst>
 </file>
@@ -508,7 +422,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -540,19 +454,6 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
@@ -597,7 +498,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -630,12 +531,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="42"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF80"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -659,7 +554,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -838,191 +733,159 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="0"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="13" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="11" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="13" fillId="4" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="11" fillId="4" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1064,7 +927,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4DD2024-5BE3-410D-830A-FD10B94659DE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66956189-047C-41E1-BC03-6CFCB70ACA6D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1243,7 +1106,7 @@
         <xdr:cNvPr id="3" name="TextBox 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EA5DF6D-828B-4D94-A781-8781B95944C7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB4920F5-902A-42C7-9638-796DD368040C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1417,15 +1280,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1904</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>287654</xdr:colOff>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>19049</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1433,7 +1296,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5524673-350E-47A1-9888-15484C7D894A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89606A3E-1711-47E2-8D32-490714300838}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1441,8 +1304,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4914899" y="666749"/>
-          <a:ext cx="6524626" cy="1905001"/>
+          <a:off x="9012554" y="828674"/>
+          <a:ext cx="6522721" cy="1905001"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1814,183 +1677,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>121943</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E516A21-7E95-4FD5-BD11-5D1477066053}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="161925" y="1943100"/>
-          <a:ext cx="5962650" cy="1419225"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent6">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="l"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>~ImpSettings </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>is used to define some settings</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> for the synchronization process</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-GB" sz="1100">
-            <a:solidFill>
-              <a:schemeClr val="dk1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>- Dummy Imports: one can control the creation of dummy imports in the table shown above. </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>These backstop dummy processes are introduced in the model in order to avoid infeasibilities that may arise if not enough energy carrier or demand can be supplied.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-GB">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr lvl="0" algn="l"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>- Vintage Bounds: VEDA can automatically generate bounds to prohibit investments in processes when a newer vintage becomes available, assuming that the last two characters of the process name are used for the first year of availability . </a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>1</xdr:row>
@@ -1999,7 +1685,7 @@
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2007,7 +1693,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDEFA196-8A04-4CC1-8339-D56C89C55A66}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7ECD8CAC-64C2-4115-80C0-C12FDE7F32F0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2293,22 +1979,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>110490</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>93345</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1412" name="Picture 2">
+        <xdr:cNvPr id="1332" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C988346D-42A0-482E-89F2-BAEFA0B3E2C2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF5A3085-D156-42B7-B3E1-C1EA3F89573B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2331,8 +2017,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="180975" y="1438275"/>
-          <a:ext cx="6134100" cy="2943225"/>
+          <a:off x="110490" y="2112645"/>
+          <a:ext cx="6290310" cy="3023235"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2367,7 +2053,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2387,7 +2073,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BF5D5C7-FB52-4EB6-BFA2-40C86434557E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD6A0440-1619-4C37-AEC0-D13D43941E5E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2819,17 +2505,17 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>476250</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
@@ -2839,7 +2525,7 @@
         <xdr:cNvPr id="3" name="TextBox 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8094662B-FE17-4939-8CEF-253A623397DC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{911031E6-05A9-4773-BB4B-FCA04CF3CAA2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2847,7 +2533,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5448300" y="323850"/>
+          <a:off x="4257675" y="323850"/>
           <a:ext cx="5962650" cy="1876425"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3111,7 +2797,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="IEA Data"/>
@@ -3246,7 +2932,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3566,13 +3252,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:J38"/>
+  <dimension ref="B3:J6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.109375" customWidth="1"/>
     <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
@@ -3581,188 +3267,51 @@
     <col min="8" max="8" width="29.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="17" t="s">
-        <v>50</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="14" t="s">
+        <v>35</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="C6" s="78" t="s">
-        <v>79</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
+        <v>35</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="62" t="s">
+        <v>60</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -3776,147 +3325,635 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B3:D23"/>
+  <dimension ref="B3:L68"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" customWidth="1"/>
+    <col min="3" max="3" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" customWidth="1"/>
+    <col min="7" max="7" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>2005</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="79" t="s">
-        <v>80</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="16">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="G12" s="65" t="s">
+        <v>95</v>
+      </c>
+      <c r="H12" s="65" t="s">
+        <v>96</v>
+      </c>
+      <c r="I12" s="65" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="13">
         <v>1</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13" s="13">
         <v>1</v>
       </c>
-      <c r="D13" s="16">
+      <c r="E13" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="16">
+      <c r="F13" s="13">
+        <v>1</v>
+      </c>
+      <c r="G13" s="13">
+        <v>1</v>
+      </c>
+      <c r="H13" s="13">
+        <v>1</v>
+      </c>
+      <c r="I13" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="13">
         <v>2</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C14" s="13">
         <v>2</v>
       </c>
-      <c r="D14" s="16">
+      <c r="E14" s="13">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="16"/>
-      <c r="C15" s="16">
+      <c r="F14" s="13">
+        <v>2</v>
+      </c>
+      <c r="G14" s="13">
+        <v>2</v>
+      </c>
+      <c r="H14" s="13">
+        <v>1</v>
+      </c>
+      <c r="I14" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="13"/>
+      <c r="C15" s="13">
         <v>5</v>
       </c>
-      <c r="D15" s="16">
+      <c r="E15" s="13">
+        <v>6</v>
+      </c>
+      <c r="F15" s="13">
+        <v>7</v>
+      </c>
+      <c r="G15" s="13">
+        <v>7</v>
+      </c>
+      <c r="H15" s="13">
+        <v>1</v>
+      </c>
+      <c r="I15" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="16"/>
-      <c r="C16" s="16">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="13"/>
+      <c r="C16" s="13">
         <v>5</v>
       </c>
-      <c r="D16" s="16">
+      <c r="E16" s="13">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="16"/>
-      <c r="C17" s="16">
+      <c r="F16" s="13">
+        <v>4</v>
+      </c>
+      <c r="G16" s="13">
+        <v>4</v>
+      </c>
+      <c r="H16" s="13">
+        <v>1</v>
+      </c>
+      <c r="I16" s="13">
         <v>5</v>
       </c>
-      <c r="D17" s="16">
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="13"/>
+      <c r="C17" s="13">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16">
+      <c r="E17" s="13">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16">
+      <c r="F17" s="13">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16">
+      <c r="G17" s="13">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16">
+      <c r="H17" s="13">
+        <v>1</v>
+      </c>
+      <c r="I17" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E18" s="13">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16">
+      <c r="F18" s="13">
         <v>5</v>
+      </c>
+      <c r="H18" s="13">
+        <v>1</v>
+      </c>
+      <c r="I18" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E19" s="13">
+        <v>5</v>
+      </c>
+      <c r="H19" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H20" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H21" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H22" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H23" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H24" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H25" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H26" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H27" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H28" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H29" s="13"/>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B34" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B35" s="66" t="s">
+        <v>100</v>
+      </c>
+      <c r="C35" s="66" t="s">
+        <v>103</v>
+      </c>
+      <c r="D35" s="66" t="s">
+        <v>110</v>
+      </c>
+      <c r="E35" s="66" t="s">
+        <v>111</v>
+      </c>
+      <c r="F35" s="67" t="s">
+        <v>115</v>
+      </c>
+      <c r="J35" s="66" t="s">
+        <v>104</v>
+      </c>
+      <c r="K35" s="66" t="s">
+        <v>106</v>
+      </c>
+      <c r="L35" s="66" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>102</v>
+      </c>
+      <c r="C37">
+        <v>2019</v>
+      </c>
+      <c r="D37">
+        <v>2019</v>
+      </c>
+      <c r="E37">
+        <v>2019</v>
+      </c>
+      <c r="F37">
+        <v>2019</v>
+      </c>
+      <c r="J37">
+        <v>2019</v>
+      </c>
+      <c r="K37">
+        <v>2019</v>
+      </c>
+      <c r="L37">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>102</v>
+      </c>
+      <c r="C38">
+        <v>2020</v>
+      </c>
+      <c r="D38">
+        <v>2020</v>
+      </c>
+      <c r="E38">
+        <v>2020</v>
+      </c>
+      <c r="F38">
+        <v>2020</v>
+      </c>
+      <c r="J38">
+        <v>2020</v>
+      </c>
+      <c r="K38">
+        <v>2020</v>
+      </c>
+      <c r="L38">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>102</v>
+      </c>
+      <c r="C39">
+        <v>2025</v>
+      </c>
+      <c r="D39">
+        <v>2023</v>
+      </c>
+      <c r="E39">
+        <v>2021</v>
+      </c>
+      <c r="F39">
+        <v>2025</v>
+      </c>
+      <c r="J39">
+        <v>2023</v>
+      </c>
+      <c r="K39">
+        <v>2023</v>
+      </c>
+      <c r="L39">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <v>2025</v>
+      </c>
+      <c r="E40">
+        <v>2022</v>
+      </c>
+      <c r="F40">
+        <v>2030</v>
+      </c>
+      <c r="J40">
+        <v>2025</v>
+      </c>
+      <c r="K40">
+        <v>2025</v>
+      </c>
+      <c r="L40">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <v>2027</v>
+      </c>
+      <c r="E41">
+        <v>2023</v>
+      </c>
+      <c r="F41">
+        <v>2035</v>
+      </c>
+      <c r="K41">
+        <v>2027</v>
+      </c>
+      <c r="L41">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <v>2030</v>
+      </c>
+      <c r="E42">
+        <v>2024</v>
+      </c>
+      <c r="F42">
+        <v>2040</v>
+      </c>
+      <c r="K42">
+        <v>2030</v>
+      </c>
+      <c r="L42">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <v>2033</v>
+      </c>
+      <c r="E43">
+        <v>2025</v>
+      </c>
+      <c r="F43">
+        <v>2045</v>
+      </c>
+      <c r="K43">
+        <v>2033</v>
+      </c>
+      <c r="L43">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <v>2035</v>
+      </c>
+      <c r="E44">
+        <v>2026</v>
+      </c>
+      <c r="F44">
+        <v>2050</v>
+      </c>
+      <c r="K44">
+        <v>2035</v>
+      </c>
+      <c r="L44">
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <v>2037</v>
+      </c>
+      <c r="E45">
+        <v>2027</v>
+      </c>
+      <c r="K45">
+        <v>2037</v>
+      </c>
+      <c r="L45">
+        <v>2027</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <v>2040</v>
+      </c>
+      <c r="E46">
+        <v>2028</v>
+      </c>
+      <c r="K46">
+        <v>2040</v>
+      </c>
+      <c r="L46">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <v>2043</v>
+      </c>
+      <c r="E47">
+        <v>2029</v>
+      </c>
+      <c r="L47">
+        <v>2029</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D48">
+        <v>2045</v>
+      </c>
+      <c r="E48">
+        <v>2030</v>
+      </c>
+      <c r="L48">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="49" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D49">
+        <v>2047</v>
+      </c>
+      <c r="E49">
+        <v>2031</v>
+      </c>
+      <c r="L49">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="50" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D50">
+        <v>2050</v>
+      </c>
+      <c r="E50">
+        <v>2032</v>
+      </c>
+      <c r="L50">
+        <v>2032</v>
+      </c>
+    </row>
+    <row r="51" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E51">
+        <v>2033</v>
+      </c>
+      <c r="L51">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="52" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E52">
+        <v>2034</v>
+      </c>
+      <c r="L52">
+        <v>2034</v>
+      </c>
+    </row>
+    <row r="53" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E53">
+        <v>2035</v>
+      </c>
+      <c r="L53">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="54" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E54">
+        <v>2036</v>
+      </c>
+      <c r="L54">
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="55" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E55">
+        <v>2037</v>
+      </c>
+      <c r="L55">
+        <v>2037</v>
+      </c>
+    </row>
+    <row r="56" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E56">
+        <v>2038</v>
+      </c>
+      <c r="L56">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="57" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E57">
+        <v>2039</v>
+      </c>
+      <c r="L57">
+        <v>2039</v>
+      </c>
+    </row>
+    <row r="58" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E58">
+        <v>2040</v>
+      </c>
+      <c r="L58">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="59" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E59">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="60" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E60">
+        <v>2042</v>
+      </c>
+    </row>
+    <row r="61" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E61">
+        <v>2043</v>
+      </c>
+    </row>
+    <row r="62" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E62">
+        <v>2044</v>
+      </c>
+    </row>
+    <row r="63" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E63">
+        <v>2045</v>
+      </c>
+    </row>
+    <row r="64" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E64">
+        <v>2046</v>
+      </c>
+    </row>
+    <row r="65" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E65">
+        <v>2047</v>
+      </c>
+    </row>
+    <row r="66" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E66">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="67" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E67">
+        <v>2049</v>
+      </c>
+    </row>
+    <row r="68" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E68">
+        <v>2050</v>
       </c>
     </row>
   </sheetData>
@@ -3929,92 +3966,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B3:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="B3:F35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="C9" sqref="C9:E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2.44140625" customWidth="1"/>
-    <col min="2" max="2" width="52.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="75" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" s="74" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="76" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="77" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="77">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="C9" s="16">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
-  <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B3:F37"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" customWidth="1"/>
     <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5546875" customWidth="1"/>
@@ -4025,32 +3987,32 @@
   <sheetData>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="E4" s="82" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="20" t="s">
-        <v>122</v>
+      <c r="B5" t="s">
+        <v>105</v>
       </c>
       <c r="C5" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -4060,13 +4022,13 @@
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="D6" s="20">
+      <c r="B6" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="14">
         <v>0</v>
       </c>
       <c r="E6">
@@ -4074,77 +4036,102 @@
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="D7" s="20">
+      <c r="B7" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="14">
         <v>0</v>
       </c>
       <c r="E7">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="D8" s="14">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C9" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D9" s="14">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B28" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B30" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B32" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
+        <v>25</v>
+      </c>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+      <c r="B34" t="s">
         <v>3</v>
       </c>
-      <c r="C36" s="6">
+      <c r="C34">
         <v>2222</v>
       </c>
-      <c r="D36" t="s">
-        <v>17</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="D34" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>3</v>
       </c>
-      <c r="C37" s="6">
+      <c r="C35">
         <v>8888</v>
       </c>
-      <c r="D37" t="s">
-        <v>17</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="D35" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4157,392 +4144,317 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="B3:H33"/>
+  <dimension ref="B3:G33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="B9" sqref="B9:E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="12"/>
-    <col min="2" max="2" width="12.109375" style="12" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" style="12" customWidth="1"/>
-    <col min="4" max="4" width="14" style="12" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" style="12" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="12"/>
+    <col min="1" max="1" width="9.109375" style="9"/>
+    <col min="2" max="2" width="12.109375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="14" style="9" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" style="9" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="9"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>2</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D7" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" s="18">
-        <v>2005</v>
-      </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D8" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" s="18">
-        <v>0.05</v>
-      </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="72" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" s="72"/>
-      <c r="D9" s="72" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" s="73">
-        <f>C23</f>
-        <v>0.24971461187214614</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="72" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" s="72"/>
-      <c r="D10" s="72" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" s="73">
-        <f>D23</f>
-        <v>0.22973744292237441</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="72" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" s="72"/>
-      <c r="D11" s="72" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="73">
-        <f>E23</f>
-        <v>0.24942922374429224</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" s="73">
-        <f>F23</f>
-        <v>0.27111872146118721</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D7" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="9">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E9" s="15"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E10" s="15"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E11" s="15"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E12" s="15"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13"/>
       <c r="C13"/>
-      <c r="D13" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="E13" s="18"/>
-      <c r="F13" s="19">
-        <v>0.9</v>
-      </c>
-      <c r="G13" s="19">
-        <v>0.95</v>
-      </c>
-      <c r="H13" s="12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F13" s="15"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14"/>
       <c r="C14"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15"/>
       <c r="C15"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17"/>
       <c r="C17"/>
       <c r="D17"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18"/>
       <c r="C18"/>
       <c r="D18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B19" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
+      <c r="B19" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="19"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="26"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="E21" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="F21" s="32" t="s">
-        <v>62</v>
+      <c r="B21" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" s="25" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="24" x14ac:dyDescent="0.25">
-      <c r="B22" s="33"/>
-      <c r="C22" s="34" t="s">
-        <v>63</v>
-      </c>
-      <c r="D22" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="E22" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="F22" s="36" t="s">
-        <v>66</v>
+      <c r="B22" s="26"/>
+      <c r="C22" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" s="29" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="C23" s="37">
+      <c r="B23" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="30">
         <f>C32/$F32*$E27</f>
         <v>0.24971461187214614</v>
       </c>
-      <c r="D23" s="38">
+      <c r="D23" s="31">
         <f>D32/$F32*$E27</f>
         <v>0.22973744292237441</v>
       </c>
-      <c r="E23" s="38">
+      <c r="E23" s="31">
         <f>C33/$F33*$E28</f>
         <v>0.24942922374429224</v>
       </c>
-      <c r="F23" s="39">
+      <c r="F23" s="32">
         <f>D33/$F33*$E28</f>
         <v>0.27111872146118721</v>
       </c>
-      <c r="G23" s="40">
+      <c r="G23" s="33">
         <f>SUM(C23:F23)</f>
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="41"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="42"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="42"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="44"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="44"/>
-      <c r="C26" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="D26" s="46" t="s">
-        <v>68</v>
-      </c>
-      <c r="E26" s="47" t="s">
-        <v>69</v>
-      </c>
-      <c r="F26" s="48"/>
-      <c r="G26" s="44"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="F26" s="39"/>
+      <c r="G26" s="34"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="49" t="s">
-        <v>70</v>
-      </c>
-      <c r="C27" s="50" t="s">
-        <v>71</v>
-      </c>
-      <c r="D27" s="51">
+      <c r="B27" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" s="42">
         <v>175</v>
       </c>
-      <c r="E27" s="52">
+      <c r="E27" s="43">
         <f>D27/D29</f>
         <v>0.47945205479452052</v>
       </c>
-      <c r="F27" s="53"/>
-      <c r="G27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="34"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="54" t="s">
-        <v>72</v>
-      </c>
-      <c r="C28" s="55" t="s">
-        <v>73</v>
-      </c>
-      <c r="D28" s="56">
+      <c r="B28" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="47">
         <f>365-D27</f>
         <v>190</v>
       </c>
-      <c r="E28" s="57">
+      <c r="E28" s="48">
         <f>D28/D29</f>
         <v>0.52054794520547942</v>
       </c>
-      <c r="F28" s="53"/>
-      <c r="G28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="34"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="42"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="58">
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="49">
         <f>SUM(D27:D28)</f>
         <v>365</v>
       </c>
-      <c r="E29" s="59">
+      <c r="E29" s="50">
         <f>SUM(E27:E28)</f>
         <v>1</v>
       </c>
-      <c r="F29" s="60"/>
-      <c r="G29" s="44"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="34"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="42"/>
-      <c r="C30" s="44"/>
-      <c r="D30" s="61"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="44"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="34"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="62"/>
-      <c r="C31" s="63" t="s">
-        <v>74</v>
-      </c>
-      <c r="D31" s="47" t="s">
-        <v>75</v>
-      </c>
-      <c r="E31" s="64"/>
-      <c r="F31" s="44"/>
-      <c r="G31" s="44"/>
+      <c r="B31" s="53"/>
+      <c r="C31" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="E31" s="55"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="34"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="65" t="s">
-        <v>71</v>
-      </c>
-      <c r="C32" s="66">
+      <c r="B32" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="57">
         <v>12.5</v>
       </c>
-      <c r="D32" s="67">
+      <c r="D32" s="58">
         <v>11.5</v>
       </c>
-      <c r="E32" s="60"/>
-      <c r="F32" s="68">
+      <c r="E32" s="51"/>
+      <c r="F32" s="51">
         <f>SUM(C32:E32)</f>
         <v>24</v>
       </c>
-      <c r="G32" s="44"/>
+      <c r="G32" s="34"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="69" t="s">
-        <v>76</v>
-      </c>
-      <c r="C33" s="70">
+      <c r="B33" s="59" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="60">
         <v>11.5</v>
       </c>
-      <c r="D33" s="71">
+      <c r="D33" s="61">
         <v>12.5</v>
       </c>
-      <c r="E33" s="60"/>
-      <c r="F33" s="60">
+      <c r="E33" s="51"/>
+      <c r="F33" s="51">
         <f>SUM(C33:E33)</f>
         <v>24</v>
       </c>
-      <c r="G33" s="44"/>
+      <c r="G33" s="34"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -4553,334 +4465,277 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="B2:I32"/>
+  <dimension ref="B2:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="F3" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="G3" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="H3" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="I3" s="22" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="20" t="s">
-        <v>93</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="I4" s="17" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="G5" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="H5" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="I5" s="17" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
+        <v>33</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" t="s">
-        <v>53</v>
-      </c>
-      <c r="G6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H6" t="s">
-        <v>53</v>
-      </c>
-      <c r="I6" s="17" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="6"/>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="C14" t="s">
-        <v>98</v>
-      </c>
-      <c r="D14" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="D14" s="63">
+        <v>1055.55</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="80">
-        <v>1055.55</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="D15" s="63">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" s="80">
-        <v>3.6</v>
+        <v>72</v>
+      </c>
+      <c r="D16" s="63">
+        <v>1000</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="C17" t="s">
-        <v>103</v>
-      </c>
-      <c r="D17" s="80">
+        <v>74</v>
+      </c>
+      <c r="D17" s="63">
         <v>1000</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="C18" t="s">
-        <v>105</v>
-      </c>
-      <c r="D18" s="80">
-        <v>1000</v>
+        <v>38</v>
+      </c>
+      <c r="D18" s="63">
+        <v>1.05555</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="80">
-        <v>1.05555</v>
+        <v>38</v>
+      </c>
+      <c r="D19" s="63">
+        <v>4.1868000000000002E-2</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>107</v>
+        <v>77</v>
       </c>
       <c r="C20" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" s="80">
-        <v>4.1868000000000002E-2</v>
+        <v>38</v>
+      </c>
+      <c r="D20" s="63">
+        <v>41.868000000000002</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>108</v>
+        <v>78</v>
       </c>
       <c r="C21" t="s">
-        <v>53</v>
-      </c>
-      <c r="D21" s="80">
-        <v>41.868000000000002</v>
+        <v>38</v>
+      </c>
+      <c r="D21" s="64">
+        <v>3.5999999999999999E-3</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="C22" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="81">
-        <v>3.5999999999999999E-3</v>
+        <v>72</v>
+      </c>
+      <c r="D22" s="63">
+        <v>1000000</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="C23" t="s">
-        <v>103</v>
-      </c>
-      <c r="D23" s="80">
-        <v>1000000</v>
+        <v>81</v>
+      </c>
+      <c r="D23" s="63">
+        <v>1000</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>111</v>
+        <v>82</v>
       </c>
       <c r="C24" t="s">
-        <v>112</v>
-      </c>
-      <c r="D24" s="80">
-        <v>1000</v>
+        <v>83</v>
+      </c>
+      <c r="D24" s="63">
+        <v>0.15384600000000001</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>113</v>
+        <v>84</v>
       </c>
       <c r="C25" t="s">
-        <v>114</v>
-      </c>
-      <c r="D25" s="80">
-        <v>0.15384600000000001</v>
+        <v>85</v>
+      </c>
+      <c r="D25" s="63">
+        <v>-1E-3</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>115</v>
+        <v>86</v>
       </c>
       <c r="C26" t="s">
-        <v>116</v>
-      </c>
-      <c r="D26" s="80">
-        <v>-1E-3</v>
+        <v>38</v>
+      </c>
+      <c r="D26" s="63">
+        <v>1000</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>117</v>
+        <v>87</v>
       </c>
       <c r="C27" t="s">
-        <v>53</v>
-      </c>
-      <c r="D27" s="80">
-        <v>1000</v>
+        <v>38</v>
+      </c>
+      <c r="D27" s="63">
+        <v>37.681199999999997</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>118</v>
+        <v>88</v>
       </c>
       <c r="C28" t="s">
-        <v>53</v>
-      </c>
-      <c r="D28" s="80">
-        <v>37.681199999999997</v>
+        <v>38</v>
+      </c>
+      <c r="D28" s="63">
+        <v>2299</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>119</v>
+        <v>89</v>
       </c>
       <c r="C29" t="s">
-        <v>53</v>
-      </c>
-      <c r="D29" s="80">
-        <v>2299</v>
+        <v>83</v>
+      </c>
+      <c r="D29" s="63">
+        <v>2.7777769999999999</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="C30" t="s">
-        <v>114</v>
-      </c>
-      <c r="D30" s="80">
-        <v>2.7777769999999999</v>
+        <v>38</v>
+      </c>
+      <c r="D30" s="63">
+        <v>3.6</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>121</v>
+        <v>38</v>
       </c>
       <c r="C31" t="s">
-        <v>53</v>
-      </c>
-      <c r="D31" s="80">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>53</v>
-      </c>
-      <c r="C32" t="s">
-        <v>53</v>
-      </c>
-      <c r="D32" s="80">
+        <v>38</v>
+      </c>
+      <c r="D31" s="63">
         <v>1</v>
       </c>
     </row>
@@ -4889,106 +4744,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="B1:I7"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3.109375" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.33203125" customWidth="1"/>
-    <col min="9" max="11" width="11.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-    </row>
-    <row r="2" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-    </row>
-    <row r="4" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-    </row>
-    <row r="5" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="0" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>